<commit_message>
Added more plot methods and properties for base
</commit_message>
<xml_diff>
--- a/Results/2021.03.12-22.39-Ref. Temperature.xlsx
+++ b/Results/2021.03.12-22.39-Ref. Temperature.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9381dc84cc5fa801/Documents/Python/Diplomatiki/Results/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_E53D268975F66FFC05FC9890E25EF23117910CA8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07FC7511-21E3-49B4-A601-BFD0876E6413}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>L_D</t>
   </si>
@@ -53,13 +47,25 @@
   </si>
   <si>
     <t>s_l</t>
+  </si>
+  <si>
+    <t>Cp_base</t>
+  </si>
+  <si>
+    <t>P_base</t>
+  </si>
+  <si>
+    <t>D_base</t>
+  </si>
+  <si>
+    <t>S_base</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,14 +102,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -150,7 +148,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -182,27 +180,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,24 +214,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -427,167 +389,221 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>3.997211972455144</v>
+        <v>3.997212021557795</v>
       </c>
       <c r="C1">
-        <v>3.372450880574513</v>
+        <v>3.3711028133256</v>
       </c>
       <c r="D1">
-        <v>3.6157965857136598</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.614855494484687</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3217126.1154598398</v>
+        <v>3217126.138732513</v>
       </c>
       <c r="C2">
-        <v>3202389.8560427539</v>
+        <v>3202355.757565538</v>
       </c>
       <c r="D2">
-        <v>3208620.315782316</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3208599.328284424</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>804842.50963649433</v>
+        <v>804842.5055718543</v>
       </c>
       <c r="C3">
-        <v>949573.46139233082</v>
+        <v>949943.0705307999</v>
       </c>
       <c r="D3">
-        <v>887389.60827051639</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>887614.8253173321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>9.6652263464689137E-2</v>
+        <v>0.09665226416387108</v>
       </c>
       <c r="C4">
-        <v>9.6209541365353382E-2</v>
+        <v>0.09620851694328061</v>
       </c>
       <c r="D4">
-        <v>9.6396723345369792E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.09639609281703397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2.4179919436527642E-2</v>
+        <v>0.02417991931441348</v>
       </c>
       <c r="C5">
-        <v>2.8528077879362221E-2</v>
+        <v>0.02853918206320463</v>
       </c>
       <c r="D5">
-        <v>2.665988560480476E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.02666665181059351</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>2627.9369309898411</v>
+        <v>2627.936930989841</v>
       </c>
       <c r="C6">
-        <v>2627.9369309898411</v>
+        <v>2627.936930989841</v>
       </c>
       <c r="D6">
-        <v>2627.9369309898411</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2627.936930989841</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>10777.645200690829</v>
+        <v>10777.64271445416</v>
       </c>
       <c r="C7">
-        <v>10777.645200690829</v>
+        <v>10777.64271445416</v>
       </c>
       <c r="D7">
-        <v>10777.645200690829</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10777.64271445416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>8.0002116246690305E-2</v>
+        <v>0.08000209779143486</v>
       </c>
       <c r="C8">
-        <v>8.0002116246690305E-2</v>
+        <v>0.08000209779143486</v>
       </c>
       <c r="D8">
-        <v>8.0002116246690305E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.08000209779143486</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>33.195353512213117</v>
+        <v>33.19535351221312</v>
       </c>
       <c r="C9">
-        <v>33.195353512213117</v>
+        <v>33.19535351221312</v>
       </c>
       <c r="D9">
-        <v>33.195353512213117</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>33.19535351221312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>79.999947606093841</v>
+        <v>79.99994760609384</v>
       </c>
       <c r="C10">
-        <v>79.999947606093841</v>
+        <v>79.99994760609384</v>
       </c>
       <c r="D10">
-        <v>79.999947606093841</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>79.99994760609384</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.41494219065819149</v>
+        <v>0.4149421906581915</v>
       </c>
       <c r="C11">
-        <v>0.41494219065819149</v>
+        <v>0.4149421906581915</v>
       </c>
       <c r="D11">
-        <v>0.41494219065819149</v>
+        <v>0.4149421906581915</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>-0.04297219340437737</v>
+      </c>
+      <c r="C12">
+        <v>-0.04297219340437737</v>
+      </c>
+      <c r="D12">
+        <v>-0.04297219340437737</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>179.4863027032873</v>
+      </c>
+      <c r="C13">
+        <v>179.4863027032873</v>
+      </c>
+      <c r="D13">
+        <v>179.4863027032873</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>37052.9710246601</v>
+      </c>
+      <c r="C14">
+        <v>37052.9710246601</v>
+      </c>
+      <c r="D14">
+        <v>37052.9710246601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>206.4389898649435</v>
+      </c>
+      <c r="C15">
+        <v>206.4389898649435</v>
+      </c>
+      <c r="D15">
+        <v>206.4389898649435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>